<commit_message>
new page created, new test added
</commit_message>
<xml_diff>
--- a/data/TestCasesVivify.xlsx
+++ b/data/TestCasesVivify.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" activeTab="1"/>
+    <workbookView windowWidth="19890" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="LogIn" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateGallery" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -111,6 +112,9 @@
   </si>
   <si>
     <t>jelena789</t>
+  </si>
+  <si>
+    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=2&amp;iurl=https%3A%2F%2Fevrobook.rs%2Ffajlovi%2Fproduct%2Fpun-mesec-looney-tunes-avanture-sasave-druzine-pun-mesec-rgb_5d83155edc58e.jpg&amp;action=click</t>
   </si>
 </sst>
 </file>
@@ -118,10 +122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -132,6 +136,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
@@ -141,9 +153,55 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,46 +212,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,77 +228,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,25 +296,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,151 +464,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,32 +490,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,15 +510,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,8 +532,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,8 +541,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -606,138 +610,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,53 +806,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1337945</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10262870" y="3685540"/>
-          <a:ext cx="6929755" cy="3896360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1108,7 +1068,7 @@
   <sheetPr/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1257,7 +1217,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1266,14 +1225,14 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1289,4 +1248,39 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=2&amp;iurl=https%3A%2F%2Fevrobook.rs%2Ffajlovi%2Fproduct%2Fpun-mesec-looney-tunes-avanture-sasave-druzine-pun-mesec-rgb_5d83155edc58e.jpg&amp;action=click"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
editing gallery test cases update
</commit_message>
<xml_diff>
--- a/data/TestCasesVivify.xlsx
+++ b/data/TestCasesVivify.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="19890" windowHeight="7665"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Editing gallery" sheetId="1" r:id="rId1"/>
     <sheet name="LogIn" sheetId="2" r:id="rId2"/>
     <sheet name="CreateGallery" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -96,25 +96,97 @@
     <t>Click on Description field</t>
   </si>
   <si>
+    <t>Description field is empty</t>
+  </si>
+  <si>
     <t>Enter description</t>
   </si>
   <si>
     <t>Pun mesec</t>
   </si>
   <si>
+    <t>Description added</t>
+  </si>
+  <si>
     <t>#3</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify editing gallery </t>
+    <t>Verify editing gallery description when there is description</t>
+  </si>
+  <si>
+    <t>Old description displayed</t>
+  </si>
+  <si>
+    <t>Delete description</t>
+  </si>
+  <si>
+    <t>Enter new description</t>
+  </si>
+  <si>
+    <t>Nocna straza</t>
+  </si>
+  <si>
+    <t>New description added</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>Verify adding image</t>
+  </si>
+  <si>
+    <t>Click on Add image</t>
+  </si>
+  <si>
+    <t>Field with Image URL is displayed</t>
+  </si>
+  <si>
+    <t>Enter Image URL</t>
+  </si>
+  <si>
+    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=2&amp;iurl=https%3A%2F%2Fevrobook.rs%2Ffajlovi%2Fproduct%2Fpun-mesec-looney-tunes-avanture-sasave-druzine-pun-mesec-rgb_5d83155edc58e.jpg&amp;action=click</t>
+  </si>
+  <si>
+    <t>Click on "Submit"</t>
+  </si>
+  <si>
+    <t>New image is visible</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>Verify adding multiple images</t>
+  </si>
+  <si>
+    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=8&amp;iurl=https%3A%2F%2Fmesecnihoroskop.com%2Fwp-content%2Fuploads%2F2015%2F04%2Fpun-mesec-mesecni-horoskop.jpg&amp;action=click</t>
+  </si>
+  <si>
+    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=9&amp;iurl=http%3A%2F%2Fbackapalankavesti.com%2Fwp-content%2Fuploads%2F2017%2F11%2Fpun-mesec.jpg&amp;action=click</t>
+  </si>
+  <si>
+    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=18&amp;iurl=https%3A%2F%2Fwww.astrosudbina.com%2Fwp-content%2Fuploads%2F2017%2F08%2Fpun-mesec-i-mlad-mesec-2017-mesec-u-svim-vaznim-fazama-datumi-1-640x494.jpg&amp;action=click</t>
+  </si>
+  <si>
+    <t>New images are visible</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Verify deleting image</t>
+  </si>
+  <si>
+    <t>Click on deleting button</t>
+  </si>
+  <si>
+    <t>Image is deleted</t>
   </si>
   <si>
     <t>jelenasabo789@gmail.com</t>
   </si>
   <si>
     <t>jelena789</t>
-  </si>
-  <si>
-    <t>https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=2&amp;iurl=https%3A%2F%2Fevrobook.rs%2Ffajlovi%2Fproduct%2Fpun-mesec-looney-tunes-avanture-sasave-druzine-pun-mesec-rgb_5d83155edc58e.jpg&amp;action=click</t>
   </si>
 </sst>
 </file>
@@ -122,10 +194,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -151,6 +223,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -161,9 +254,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,21 +268,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -205,13 +283,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -228,6 +299,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -242,6 +321,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -250,8 +336,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,7 +346,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,21 +354,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,13 +368,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,169 +434,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,15 +559,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -510,6 +573,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,8 +604,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,8 +613,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,15 +664,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -613,127 +685,127 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1066,10 +1138,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1161,7 +1233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1174,47 +1246,318 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="4:4">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="4:4">
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
       <c r="D10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="4:4">
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
       <c r="D11" t="s">
         <v>25</v>
       </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="4:5">
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
       <c r="D13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6">
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5">
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6">
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="D33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6">
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6">
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6">
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6">
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6">
+      <c r="D45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6">
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6">
+      <c r="D47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E28" r:id="rId1" display="https://images.search.yahoo.com/search/images;_ylt=A2KLfSXnnzxgAwUAMz9XNyoA;_ylu=Y29sbwNiZjEEcG9zAzEEdnRpZANERkQ2XzEEc2VjA3BpdnM-?p=pun+mesec&amp;fr2=piv-web&amp;fr=mcafee#id=2&amp;iurl=https%3A%2F%2Fevrobook.rs%2Ffajlovi%2Fproduct%2Fpun-mesec-looney-tunes-avanture-sasave-druzine-pun-mesec-rgb_5d83155edc58e.jpg&amp;action=click"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1233,12 +1576,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1268,12 +1611,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>